<commit_message>
open mysql test classes
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/prepareStatement/sql_ps_dql_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/prepareStatement/sql_ps_dql_cases.xlsx
@@ -253,7 +253,7 @@
     <t>src/test/resources/io.dingodb.test/testdata/cases/prepareStatement/expectedresult/ps_dql_008.csv</t>
   </si>
   <si>
-    <t>Double,Double</t>
+    <t>Float,Float</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -629,7 +629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>

</xml_diff>